<commit_message>
Section6. How to use Column & Row Widgets for Layout
</commit_message>
<xml_diff>
--- a/학점은행/2022 1학기/학점은행시간표2.xlsx
+++ b/학점은행/2022 1학기/학점은행시간표2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjwhd\git\TIL\학점은행\2022 1학기\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7815A9A5-F67A-4449-9EDF-1446055B75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3288B1A-092E-46FD-9937-8C559DA9BF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{0B5A47C8-42F4-4ED1-BB40-2F999C7C333D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -602,7 +602,9 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -646,7 +648,9 @@
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>

</xml_diff>

<commit_message>
Flutter Slider Widget, Customising Widgets, First Order Objects
</commit_message>
<xml_diff>
--- a/학점은행/2022 1학기/학점은행시간표2.xlsx
+++ b/학점은행/2022 1학기/학점은행시간표2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjwhd\git\TIL\학점은행\2022 1학기\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A823AFB-01BA-4DD4-A6C5-2EC91DFB3121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3CF87F-D523-4C8F-BC7D-1615760DC095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="510" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{0B5A47C8-42F4-4ED1-BB40-2F999C7C333D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -716,7 +716,9 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -742,7 +744,9 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -768,7 +772,9 @@
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>

</xml_diff>

<commit_message>
Flutter-Async Challenge And About Api
</commit_message>
<xml_diff>
--- a/학점은행/2022 1학기/학점은행시간표2.xlsx
+++ b/학점은행/2022 1학기/학점은행시간표2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjwhd\git\TIL\학점은행\2022 1학기\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A52893-F4DF-4824-9E72-6E67E1566011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47C8A14-6026-43BA-BDBF-9325ED5D49E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{0B5A47C8-42F4-4ED1-BB40-2F999C7C333D}"/>
+    <workbookView xWindow="3600" yWindow="4185" windowWidth="21600" windowHeight="11070" xr2:uid="{0B5A47C8-42F4-4ED1-BB40-2F999C7C333D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -695,7 +695,9 @@
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -779,7 +781,9 @@
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>

</xml_diff>

<commit_message>
Flutter-BitcoinChallenge, About Material and Cupertino
</commit_message>
<xml_diff>
--- a/학점은행/2022 1학기/학점은행시간표2.xlsx
+++ b/학점은행/2022 1학기/학점은행시간표2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjwhd\git\TIL\학점은행\2022 1학기\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E38B7D6-D71A-4E12-A308-09F34923E06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADDA5D6-B5C4-4D96-B2B9-9AE24ED9B236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="4185" windowWidth="21600" windowHeight="11070" xr2:uid="{0B5A47C8-42F4-4ED1-BB40-2F999C7C333D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -674,7 +674,9 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -794,7 +796,9 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>

</xml_diff>

<commit_message>
Webhaking Xss, Cookie, mango
</commit_message>
<xml_diff>
--- a/학점은행/2022 1학기/학점은행시간표2.xlsx
+++ b/학점은행/2022 1학기/학점은행시간표2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjwhd\git\TIL\학점은행\2022 1학기\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADDA5D6-B5C4-4D96-B2B9-9AE24ED9B236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31D1A74-667D-4DE3-933A-543901503190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="4185" windowWidth="21600" windowHeight="11070" xr2:uid="{0B5A47C8-42F4-4ED1-BB40-2F999C7C333D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -614,7 +614,9 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -644,7 +646,9 @@
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -706,7 +710,9 @@
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -736,7 +742,9 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -766,7 +774,9 @@
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -828,7 +838,9 @@
       <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>

</xml_diff>